<commit_message>
Info completa máquina 2
</commit_message>
<xml_diff>
--- a/Docs/Tablas Lab 4 - Maquina2.xlsx
+++ b/Docs/Tablas Lab 4 - Maquina2.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Documents\Tareas\ESTRUC. DE DATOS Y ALGORITMOS\lab4\LabSorts-S04-G09\Docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lauda\Documents\UniAndes\2do semestre\Estructuras de Datos y Algoritmos\Lab 4\LabSorts-S04-G09\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76952C34-2116-484D-AB7E-15A5B00D7539}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DE51919-5479-43A0-B9B2-1FB357FE1819}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6375" yWindow="2265" windowWidth="21600" windowHeight="11505" xr2:uid="{D82936D8-D2C9-4EB2-9CBC-3665F65B95FD}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="1" activeTab="5" xr2:uid="{D82936D8-D2C9-4EB2-9CBC-3665F65B95FD}"/>
   </bookViews>
   <sheets>
     <sheet name="Datos Lab4" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <r>
       <t>T</t>
@@ -56,15 +56,6 @@
     </r>
   </si>
   <si>
-    <t>Insertion Sort [ms]</t>
-  </si>
-  <si>
-    <t>Selection Sort [ms]</t>
-  </si>
-  <si>
-    <t>Shell Sort [ms]</t>
-  </si>
-  <si>
     <r>
       <t>T</t>
     </r>
@@ -79,12 +70,30 @@
       <t>amaño de la muestra (ARRAYLIST)</t>
     </r>
   </si>
+  <si>
+    <t>(L)Insertion Sort [ms]</t>
+  </si>
+  <si>
+    <t>(A)Insertion Sort [ms]</t>
+  </si>
+  <si>
+    <t>(A)Selection Sort [ms]</t>
+  </si>
+  <si>
+    <t>(A)Shell Sort [ms]</t>
+  </si>
+  <si>
+    <t>(L)Selection Sort [ms]</t>
+  </si>
+  <si>
+    <t>(L)Shell Sort [ms]</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -109,16 +118,40 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Dax-Regular"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Dax-Regular"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCCCCCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -126,11 +159,29 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color rgb="FF666666"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FF666666"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -144,11 +195,150 @@
     <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="4" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="5" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="5" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="12">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Dax-Regular"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Dax-Regular"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Dax-Regular"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Dax-Regular"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Dax-Regular"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -308,129 +498,6 @@
         <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="11"/>
-        <color theme="1"/>
-        <name val="Dax-Regular"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Dax-Regular"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Dax-Regular"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Dax-Regular"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Dax-Regular"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
         <color rgb="FF000000"/>
         <name val="Dax-Regular"/>
         <scheme val="none"/>
@@ -459,7 +526,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="es-ES"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -526,7 +593,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="es-CO"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -545,7 +612,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Insertion Sort [ms]</c:v>
+                  <c:v>(A)Insertion Sort [ms]</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -588,6 +655,12 @@
             <c:dispRSqr val="1"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-0.71299658982424052"/>
+                  <c:y val="0.29728519875826048"/>
+                </c:manualLayout>
+              </c:layout>
               <c:numFmt formatCode="General" sourceLinked="0"/>
               <c:spPr>
                 <a:noFill/>
@@ -613,7 +686,7 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="en-US"/>
+                  <a:endParaRPr lang="es-CO"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
@@ -661,37 +734,25 @@
             <c:numRef>
               <c:f>'Datos Lab4'!$B$2:$B$11</c:f>
               <c:numCache>
-                <c:formatCode>0.00</c:formatCode>
+                <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0" formatCode="General">
-                  <c:v>609.38</c:v>
+                  <c:v>906.25</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>20</c:v>
+                  <c:v>3651.0419999999999</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>30</c:v>
+                  <c:v>14911.458000000001</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>40</c:v>
+                  <c:v>63177.082999999999</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>50</c:v>
+                  <c:v>249260.41699999999</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>60</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>70</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>80</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>90</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>100</c:v>
+                  <c:v>1037869.791</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -712,7 +773,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Selection Sort [ms]</c:v>
+                  <c:v>(A)Selection Sort [ms]</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -751,11 +812,16 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
-            <c:trendlineType val="poly"/>
-            <c:order val="2"/>
+            <c:trendlineType val="power"/>
             <c:dispRSqr val="1"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-0.71584003551293163"/>
+                  <c:y val="0.21983717620455245"/>
+                </c:manualLayout>
+              </c:layout>
               <c:numFmt formatCode="General" sourceLinked="0"/>
               <c:spPr>
                 <a:noFill/>
@@ -781,7 +847,7 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="en-US"/>
+                  <a:endParaRPr lang="es-CO"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
@@ -829,37 +895,25 @@
             <c:numRef>
               <c:f>'Datos Lab4'!$C$2:$C$11</c:f>
               <c:numCache>
-                <c:formatCode>0.00</c:formatCode>
+                <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0" formatCode="General">
-                  <c:v>640.63</c:v>
+                  <c:v>973.5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2</c:v>
+                  <c:v>3567.7080000000001</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>642.63</c:v>
+                  <c:v>14895.833000000001</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>644.63</c:v>
+                  <c:v>65828.125</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1287.26</c:v>
+                  <c:v>284911.45799999998</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1931.8899999999999</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>3219.1499999999996</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>5151.0399999999991</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>8370.1899999999987</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>13521.229999999998</c:v>
+                  <c:v>1090411.4580000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -880,7 +934,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Shell Sort [ms]</c:v>
+                  <c:v>(A)Shell Sort [ms]</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -919,7 +973,7 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
-            <c:trendlineType val="log"/>
+            <c:trendlineType val="power"/>
             <c:dispRSqr val="1"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
@@ -948,7 +1002,7 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="en-US"/>
+                  <a:endParaRPr lang="es-CO"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
@@ -996,37 +1050,34 @@
             <c:numRef>
               <c:f>'Datos Lab4'!$D$2:$D$11</c:f>
               <c:numCache>
-                <c:formatCode>0.00</c:formatCode>
+                <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="10"/>
-                <c:pt idx="0" formatCode="General">
-                  <c:v>31.25</c:v>
+                <c:pt idx="0">
+                  <c:v>88.542000000000002</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>46.25</c:v>
+                  <c:v>192.708</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>56.25</c:v>
+                  <c:v>395.83300000000003</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>66.25</c:v>
+                  <c:v>1026.0419999999999</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>76.25</c:v>
+                  <c:v>2359.375</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>86.25</c:v>
+                  <c:v>5244.7920000000004</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>96.25</c:v>
+                  <c:v>8495.625</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>106.25</c:v>
+                  <c:v>31187.5</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>116.25</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>126.25</c:v>
+                  <c:v>77869.792000000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1053,6 +1104,8 @@
         <c:axId val="696671312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="512000"/>
+          <c:min val="0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
@@ -1126,7 +1179,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="es-CO"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -1164,7 +1217,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="es-CO"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1833162896"/>
@@ -1175,6 +1228,8 @@
         <c:axId val="1833162896"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="1800000"/>
+          <c:min val="0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -1248,7 +1303,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="es-CO"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -1286,7 +1341,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="es-CO"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="696671312"/>
@@ -1328,7 +1383,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="es-CO"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -1365,7 +1420,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="es-CO"/>
     </a:p>
   </c:txPr>
 </c:chartSpace>
@@ -1374,7 +1429,7 @@
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="es-ES"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1441,7 +1496,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="es-CO"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -1460,7 +1515,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Insertion Sort [ms]</c:v>
+                  <c:v>(L)Insertion Sort [ms]</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1503,6 +1558,12 @@
             <c:dispRSqr val="1"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-0.73486924896801842"/>
+                  <c:y val="0.27426011097202296"/>
+                </c:manualLayout>
+              </c:layout>
               <c:numFmt formatCode="General" sourceLinked="0"/>
               <c:spPr>
                 <a:noFill/>
@@ -1528,7 +1589,7 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="en-US"/>
+                  <a:endParaRPr lang="es-CO"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
@@ -1576,37 +1637,13 @@
             <c:numRef>
               <c:f>'Datos Lab4'!$B$15:$B$24</c:f>
               <c:numCache>
-                <c:formatCode>0.00</c:formatCode>
+                <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>50</c:v>
+                  <c:v>124432.291</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>60</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>70</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>80</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>90</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>100</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>110</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>120</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>130</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>140</c:v>
+                  <c:v>630760.41599999997</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1627,7 +1664,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Selection Sort [ms]</c:v>
+                  <c:v>(L)Selection Sort [ms]</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1666,11 +1703,16 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
-            <c:trendlineType val="poly"/>
-            <c:order val="2"/>
+            <c:trendlineType val="power"/>
             <c:dispRSqr val="1"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-0.74033741375396289"/>
+                  <c:y val="0.35380132332447983"/>
+                </c:manualLayout>
+              </c:layout>
               <c:numFmt formatCode="General" sourceLinked="0"/>
               <c:spPr>
                 <a:noFill/>
@@ -1696,46 +1738,46 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="en-US"/>
+                  <a:endParaRPr lang="es-CO"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>'Datos Lab4'!$C$15:$C$24</c:f>
+              <c:f>'Datos Lab4'!$A$15:$A$24</c:f>
               <c:numCache>
-                <c:formatCode>0.00</c:formatCode>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>2</c:v>
+                  <c:v>1000</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4</c:v>
+                  <c:v>2000</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>6</c:v>
+                  <c:v>4000</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>10</c:v>
+                  <c:v>8000</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>16</c:v>
+                  <c:v>16000</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>26</c:v>
+                  <c:v>32000</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>42</c:v>
+                  <c:v>64000</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>68</c:v>
+                  <c:v>128000</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>110</c:v>
+                  <c:v>256000</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>178</c:v>
+                  <c:v>512000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1744,37 +1786,13 @@
             <c:numRef>
               <c:f>'Datos Lab4'!$C$15:$C$24</c:f>
               <c:numCache>
-                <c:formatCode>0.00</c:formatCode>
+                <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>2</c:v>
+                  <c:v>105270.833</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>16</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>26</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>42</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>68</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>110</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>178</c:v>
+                  <c:v>603000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1795,7 +1813,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Shell Sort [ms]</c:v>
+                  <c:v>(L)Shell Sort [ms]</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1834,10 +1852,16 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
-            <c:trendlineType val="log"/>
+            <c:trendlineType val="power"/>
             <c:dispRSqr val="1"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-0.74586026018776685"/>
+                  <c:y val="0.44590167446942996"/>
+                </c:manualLayout>
+              </c:layout>
               <c:numFmt formatCode="General" sourceLinked="0"/>
               <c:spPr>
                 <a:noFill/>
@@ -1863,7 +1887,7 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="en-US"/>
+                  <a:endParaRPr lang="es-CO"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
@@ -1911,37 +1935,19 @@
             <c:numRef>
               <c:f>'Datos Lab4'!$D$15:$D$24</c:f>
               <c:numCache>
-                <c:formatCode>0.00</c:formatCode>
+                <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>35</c:v>
+                  <c:v>6380.2079999999996</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>78</c:v>
+                  <c:v>25911.457999999999</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>88</c:v>
+                  <c:v>118604.167</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>98</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>108</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>118</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>128</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>138</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>148</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>158</c:v>
+                  <c:v>583630.20799999998</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1968,6 +1974,8 @@
         <c:axId val="696671312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="512000"/>
+          <c:min val="0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
@@ -2041,7 +2049,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="es-CO"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -2079,7 +2087,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="es-CO"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1833162896"/>
@@ -2090,6 +2098,8 @@
         <c:axId val="1833162896"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="1800000"/>
+          <c:min val="0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -2163,11 +2173,11 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="es-CO"/>
             </a:p>
           </c:txPr>
         </c:title>
-        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:numFmt formatCode="#,##0" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -2201,7 +2211,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="es-CO"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="696671312"/>
@@ -2243,7 +2253,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="es-CO"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -2280,7 +2290,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="es-CO"/>
     </a:p>
   </c:txPr>
 </c:chartSpace>
@@ -2289,7 +2299,7 @@
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="es-ES"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -2356,7 +2366,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="es-CO"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -2375,7 +2385,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Insertion Sort [ms]</c:v>
+                  <c:v>(A)Insertion Sort [ms]</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2414,11 +2424,16 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
-            <c:trendlineType val="poly"/>
-            <c:order val="2"/>
+            <c:trendlineType val="power"/>
             <c:dispRSqr val="1"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-0.71299658982424052"/>
+                  <c:y val="0.26355352756046968"/>
+                </c:manualLayout>
+              </c:layout>
               <c:numFmt formatCode="General" sourceLinked="0"/>
               <c:spPr>
                 <a:noFill/>
@@ -2444,7 +2459,7 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="en-US"/>
+                  <a:endParaRPr lang="es-CO"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
@@ -2492,37 +2507,25 @@
             <c:numRef>
               <c:f>'Datos Lab4'!$B$2:$B$11</c:f>
               <c:numCache>
-                <c:formatCode>0.00</c:formatCode>
+                <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0" formatCode="General">
-                  <c:v>609.38</c:v>
+                  <c:v>906.25</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>20</c:v>
+                  <c:v>3651.0419999999999</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>30</c:v>
+                  <c:v>14911.458000000001</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>40</c:v>
+                  <c:v>63177.082999999999</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>50</c:v>
+                  <c:v>249260.41699999999</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>60</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>70</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>80</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>90</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>100</c:v>
+                  <c:v>1037869.791</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2543,7 +2546,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Insertion Sort [ms]</c:v>
+                  <c:v>(L)Insertion Sort [ms]</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2582,11 +2585,16 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
-            <c:trendlineType val="poly"/>
-            <c:order val="2"/>
+            <c:trendlineType val="power"/>
             <c:dispRSqr val="1"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-0.7840827320415189"/>
+                  <c:y val="-3.7865803459366985E-2"/>
+                </c:manualLayout>
+              </c:layout>
               <c:numFmt formatCode="General" sourceLinked="0"/>
               <c:spPr>
                 <a:noFill/>
@@ -2612,7 +2620,7 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="en-US"/>
+                  <a:endParaRPr lang="es-CO"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
@@ -2660,37 +2668,13 @@
             <c:numRef>
               <c:f>'Datos Lab4'!$B$15:$B$24</c:f>
               <c:numCache>
-                <c:formatCode>0.00</c:formatCode>
+                <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>50</c:v>
+                  <c:v>124432.291</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>60</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>70</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>80</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>90</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>100</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>110</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>120</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>130</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>140</c:v>
+                  <c:v>630760.41599999997</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2717,6 +2701,8 @@
         <c:axId val="1328118000"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="512000"/>
+          <c:min val="0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
@@ -2790,7 +2776,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="es-CO"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -2828,7 +2814,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="es-CO"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1328121328"/>
@@ -2839,6 +2825,8 @@
         <c:axId val="1328121328"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="1800000"/>
+          <c:min val="0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -2907,7 +2895,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="es-CO"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -2945,7 +2933,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="es-CO"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1328118000"/>
@@ -2987,7 +2975,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="es-CO"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -3024,7 +3012,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="es-CO"/>
     </a:p>
   </c:txPr>
 </c:chartSpace>
@@ -3033,7 +3021,7 @@
 <file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="es-ES"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -3095,7 +3083,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="es-CO"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -3114,7 +3102,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Selection Sort [ms]</c:v>
+                  <c:v>(A)Selection Sort [ms]</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -3153,11 +3141,16 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
-            <c:trendlineType val="poly"/>
-            <c:order val="2"/>
+            <c:trendlineType val="power"/>
             <c:dispRSqr val="1"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-0.71994115910238998"/>
+                  <c:y val="0.23006249078048785"/>
+                </c:manualLayout>
+              </c:layout>
               <c:numFmt formatCode="General" sourceLinked="0"/>
               <c:spPr>
                 <a:noFill/>
@@ -3183,7 +3176,7 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="en-US"/>
+                  <a:endParaRPr lang="es-CO"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
@@ -3231,37 +3224,25 @@
             <c:numRef>
               <c:f>'Datos Lab4'!$C$2:$C$11</c:f>
               <c:numCache>
-                <c:formatCode>0.00</c:formatCode>
+                <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0" formatCode="General">
-                  <c:v>640.63</c:v>
+                  <c:v>973.5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2</c:v>
+                  <c:v>3567.7080000000001</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>642.63</c:v>
+                  <c:v>14895.833000000001</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>644.63</c:v>
+                  <c:v>65828.125</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1287.26</c:v>
+                  <c:v>284911.45799999998</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1931.8899999999999</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>3219.1499999999996</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>5151.0399999999991</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>8370.1899999999987</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>13521.229999999998</c:v>
+                  <c:v>1090411.4580000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3282,7 +3263,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Selection Sort [ms]</c:v>
+                  <c:v>(L)Selection Sort [ms]</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -3321,11 +3302,16 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
-            <c:trendlineType val="poly"/>
-            <c:order val="2"/>
+            <c:trendlineType val="power"/>
             <c:dispRSqr val="1"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-0.77998160845206055"/>
+                  <c:y val="-4.8331752453111311E-2"/>
+                </c:manualLayout>
+              </c:layout>
               <c:numFmt formatCode="General" sourceLinked="0"/>
               <c:spPr>
                 <a:noFill/>
@@ -3351,7 +3337,7 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="en-US"/>
+                  <a:endParaRPr lang="es-CO"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
@@ -3399,37 +3385,13 @@
             <c:numRef>
               <c:f>'Datos Lab4'!$C$15:$C$24</c:f>
               <c:numCache>
-                <c:formatCode>0.00</c:formatCode>
+                <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>2</c:v>
+                  <c:v>105270.833</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>16</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>26</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>42</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>68</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>110</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>178</c:v>
+                  <c:v>603000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3456,6 +3418,8 @@
         <c:axId val="1328118000"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="512000"/>
+          <c:min val="0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
@@ -3529,7 +3493,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="es-CO"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -3567,7 +3531,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="es-CO"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1328121328"/>
@@ -3578,6 +3542,8 @@
         <c:axId val="1328121328"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="1800000"/>
+          <c:min val="0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -3646,7 +3612,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="es-CO"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -3684,7 +3650,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="es-CO"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1328118000"/>
@@ -3726,7 +3692,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="es-CO"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -3763,7 +3729,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="es-CO"/>
     </a:p>
   </c:txPr>
 </c:chartSpace>
@@ -3772,7 +3738,7 @@
 <file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="es-ES"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -3834,7 +3800,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="es-CO"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -3853,7 +3819,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Shell Sort [ms]</c:v>
+                  <c:v>(A)Shell Sort [ms]</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -3892,11 +3858,16 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
-            <c:trendlineType val="poly"/>
-            <c:order val="2"/>
+            <c:trendlineType val="power"/>
             <c:dispRSqr val="1"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-1.5805579616317823E-2"/>
+                  <c:y val="-5.6310431584421061E-2"/>
+                </c:manualLayout>
+              </c:layout>
               <c:numFmt formatCode="General" sourceLinked="0"/>
               <c:spPr>
                 <a:noFill/>
@@ -3922,7 +3893,7 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="en-US"/>
+                  <a:endParaRPr lang="es-CO"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
@@ -3970,37 +3941,34 @@
             <c:numRef>
               <c:f>'Datos Lab4'!$D$2:$D$11</c:f>
               <c:numCache>
-                <c:formatCode>0.00</c:formatCode>
+                <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="10"/>
-                <c:pt idx="0" formatCode="General">
-                  <c:v>31.25</c:v>
+                <c:pt idx="0">
+                  <c:v>88.542000000000002</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>46.25</c:v>
+                  <c:v>192.708</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>56.25</c:v>
+                  <c:v>395.83300000000003</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>66.25</c:v>
+                  <c:v>1026.0419999999999</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>76.25</c:v>
+                  <c:v>2359.375</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>86.25</c:v>
+                  <c:v>5244.7920000000004</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>96.25</c:v>
+                  <c:v>8495.625</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>106.25</c:v>
+                  <c:v>31187.5</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>116.25</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>126.25</c:v>
+                  <c:v>77869.792000000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4021,7 +3989,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Shell Sort [ms]</c:v>
+                  <c:v>(L)Shell Sort [ms]</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -4060,11 +4028,16 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
-            <c:trendlineType val="poly"/>
-            <c:order val="2"/>
+            <c:trendlineType val="power"/>
             <c:dispRSqr val="1"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-0.72945576582993343"/>
+                  <c:y val="6.0911823143591998E-3"/>
+                </c:manualLayout>
+              </c:layout>
               <c:numFmt formatCode="General" sourceLinked="0"/>
               <c:spPr>
                 <a:noFill/>
@@ -4090,7 +4063,7 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="en-US"/>
+                  <a:endParaRPr lang="es-CO"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
@@ -4138,37 +4111,19 @@
             <c:numRef>
               <c:f>'Datos Lab4'!$D$15:$D$24</c:f>
               <c:numCache>
-                <c:formatCode>0.00</c:formatCode>
+                <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>35</c:v>
+                  <c:v>6380.2079999999996</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>78</c:v>
+                  <c:v>25911.457999999999</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>88</c:v>
+                  <c:v>118604.167</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>98</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>108</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>118</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>128</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>138</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>148</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>158</c:v>
+                  <c:v>583630.20799999998</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4195,6 +4150,8 @@
         <c:axId val="1328118000"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="512000"/>
+          <c:min val="0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
@@ -4268,7 +4225,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="es-CO"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -4306,7 +4263,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="es-CO"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1328121328"/>
@@ -4317,6 +4274,8 @@
         <c:axId val="1328121328"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="1800000"/>
+          <c:min val="0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -4385,11 +4344,11 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="es-CO"/>
             </a:p>
           </c:txPr>
         </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="#,##0" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -4423,7 +4382,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="es-CO"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1328118000"/>
@@ -4465,7 +4424,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="es-CO"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -4502,7 +4461,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="es-CO"/>
     </a:p>
   </c:txPr>
 </c:chartSpace>
@@ -7286,7 +7245,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{BF2A59F4-6CD8-490D-818C-7B3BB3F2B140}">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="117" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="85" workbookViewId="0"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -7297,7 +7256,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{0D09CF8B-80E2-4734-A9D4-9F6060F1BA3D}">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="117" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="90" workbookViewId="0"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -7308,7 +7267,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{3D4D373F-B89D-476A-916E-D6B8B50B0AC1}">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="117" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="85" workbookViewId="0"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -7319,7 +7278,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{662C0436-FCD4-45AD-AA7D-093158D92847}">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="117" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="85" workbookViewId="0"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -7330,7 +7289,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{39C68510-AE01-4761-A7FB-5F1B76E923F7}">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="76" workbookViewId="0" zoomToFit="1"/>
+    <sheetView tabSelected="1" zoomScale="85" workbookViewId="0"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -7341,7 +7300,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="8662051" cy="6288490"/>
+    <xdr:ext cx="9290137" cy="6067295"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
@@ -7374,7 +7333,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="8659519" cy="6284148"/>
+    <xdr:ext cx="9290137" cy="6067295"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
@@ -7407,7 +7366,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="8659519" cy="6284148"/>
+    <xdr:ext cx="9290137" cy="6067295"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
@@ -7440,7 +7399,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="8659519" cy="6284148"/>
+    <xdr:ext cx="9290137" cy="6067295"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
@@ -7473,7 +7432,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="8660230" cy="6291513"/>
+    <xdr:ext cx="9290137" cy="6067295"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
@@ -7503,33 +7462,33 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{072D0253-75B0-4C0B-8972-D03303899249}" name="Table1" displayName="Table1" ref="A1:D11" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{072D0253-75B0-4C0B-8972-D03303899249}" name="Table1" displayName="Table1" ref="A1:D11" totalsRowShown="0" headerRowDxfId="11" dataDxfId="0">
   <autoFilter ref="A1:D11" xr:uid="{B245DDE7-54F2-4A7A-AC17-5CA17DD7B03F}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{A7AF2A2F-BC4B-404E-9B8B-256DA178E68B}" name="Tamaño de la muestra (ARRAYLIST)" dataDxfId="9"/>
-    <tableColumn id="2" xr3:uid="{23CECC62-35E0-466E-9502-4F5CC2E6F7A7}" name="Insertion Sort [ms]" dataDxfId="8"/>
-    <tableColumn id="3" xr3:uid="{19B1D273-887B-4392-991E-015D36D99E5B}" name="Selection Sort [ms]" dataDxfId="7"/>
-    <tableColumn id="4" xr3:uid="{56471E76-DCC6-4EED-8237-BCC256B57E91}" name="Shell Sort [ms]" dataDxfId="6"/>
+    <tableColumn id="1" xr3:uid="{A7AF2A2F-BC4B-404E-9B8B-256DA178E68B}" name="Tamaño de la muestra (ARRAYLIST)" dataDxfId="4"/>
+    <tableColumn id="2" xr3:uid="{23CECC62-35E0-466E-9502-4F5CC2E6F7A7}" name="(A)Insertion Sort [ms]" dataDxfId="3"/>
+    <tableColumn id="3" xr3:uid="{19B1D273-887B-4392-991E-015D36D99E5B}" name="(A)Selection Sort [ms]" dataDxfId="2"/>
+    <tableColumn id="4" xr3:uid="{56471E76-DCC6-4EED-8237-BCC256B57E91}" name="(A)Shell Sort [ms]" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{C35EFFA4-2B65-46C5-8257-6884800B9577}" name="Table13" displayName="Table13" ref="A14:D24" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{C35EFFA4-2B65-46C5-8257-6884800B9577}" name="Table13" displayName="Table13" ref="A14:D24" totalsRowShown="0" headerRowDxfId="10" dataDxfId="9">
   <autoFilter ref="A14:D24" xr:uid="{5C24B5A8-1B8E-4092-B34A-66FF5413D106}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{16584851-71BC-4FF5-B248-C3F46BA653AF}" name="Tamaño de la muestra (LINKED_LIST)" dataDxfId="3"/>
-    <tableColumn id="2" xr3:uid="{4F9B7329-040C-4D35-96E7-B9181424DC65}" name="Insertion Sort [ms]" dataDxfId="2"/>
-    <tableColumn id="3" xr3:uid="{BDA028DF-4CED-4928-B040-96AD8F8A43EB}" name="Selection Sort [ms]" dataDxfId="1"/>
-    <tableColumn id="4" xr3:uid="{A5E99D51-DD73-48A7-AE0D-601A8EE89AFA}" name="Shell Sort [ms]" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{16584851-71BC-4FF5-B248-C3F46BA653AF}" name="Tamaño de la muestra (LINKED_LIST)" dataDxfId="8"/>
+    <tableColumn id="2" xr3:uid="{4F9B7329-040C-4D35-96E7-B9181424DC65}" name="(L)Insertion Sort [ms]" dataDxfId="7"/>
+    <tableColumn id="3" xr3:uid="{BDA028DF-4CED-4928-B040-96AD8F8A43EB}" name="(L)Selection Sort [ms]" dataDxfId="6"/>
+    <tableColumn id="4" xr3:uid="{A5E99D51-DD73-48A7-AE0D-601A8EE89AFA}" name="(L)Shell Sort [ms]" dataDxfId="5"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -7825,13 +7784,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5B14742-4EBB-4241-AC8A-0E5F24F7BB7B}">
-  <dimension ref="A1:D24"/>
+  <dimension ref="A1:F24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="34.140625" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="21.5703125" style="3" bestFit="1" customWidth="1"/>
@@ -7839,347 +7798,254 @@
     <col min="4" max="4" width="18" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:6" ht="30">
       <c r="A1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>2</v>
-      </c>
       <c r="D1" s="2" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:6" ht="15.75" thickBot="1">
       <c r="A2" s="1">
         <v>1000</v>
       </c>
-      <c r="B2">
-        <v>609.38</v>
+      <c r="B2" s="6">
+        <v>906.25</v>
       </c>
-      <c r="C2">
-        <v>640.63</v>
+      <c r="C2" s="6">
+        <v>973.5</v>
       </c>
-      <c r="D2">
-        <v>31.25</v>
+      <c r="D2" s="10">
+        <v>88.542000000000002</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:6" ht="16.5" thickTop="1" thickBot="1">
       <c r="A3" s="1">
         <v>2000</v>
       </c>
-      <c r="B3" s="4">
-        <v>20</v>
+      <c r="B3" s="7">
+        <v>3651.0419999999999</v>
       </c>
-      <c r="C3" s="4">
-        <v>2</v>
+      <c r="C3" s="7">
+        <v>3567.7080000000001</v>
       </c>
-      <c r="D3" s="4">
-        <f>D2+15</f>
-        <v>46.25</v>
+      <c r="D3" s="7">
+        <v>192.708</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:6" ht="15.75" thickBot="1">
       <c r="A4" s="1">
         <v>4000</v>
       </c>
-      <c r="B4" s="4">
-        <v>30</v>
+      <c r="B4" s="8">
+        <v>14911.458000000001</v>
       </c>
-      <c r="C4" s="4">
-        <f>C3+C2</f>
-        <v>642.63</v>
+      <c r="C4" s="8">
+        <v>14895.833000000001</v>
       </c>
-      <c r="D4" s="4">
-        <f t="shared" ref="D4:D11" si="0">D3+10</f>
-        <v>56.25</v>
+      <c r="D4" s="8">
+        <v>395.83300000000003</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:6" ht="15.75" thickBot="1">
       <c r="A5" s="1">
         <v>8000</v>
       </c>
-      <c r="B5" s="4">
-        <v>40</v>
+      <c r="B5" s="7">
+        <v>63177.082999999999</v>
       </c>
-      <c r="C5" s="4">
-        <f t="shared" ref="C5:C11" si="1">C4+C3</f>
-        <v>644.63</v>
+      <c r="C5" s="7">
+        <v>65828.125</v>
       </c>
-      <c r="D5" s="4">
-        <f t="shared" si="0"/>
-        <v>66.25</v>
+      <c r="D5" s="7">
+        <v>1026.0419999999999</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:6" ht="15.75" thickBot="1">
       <c r="A6" s="1">
         <v>16000</v>
       </c>
-      <c r="B6" s="4">
-        <v>50</v>
+      <c r="B6" s="8">
+        <v>249260.41699999999</v>
       </c>
-      <c r="C6" s="4">
-        <f t="shared" si="1"/>
-        <v>1287.26</v>
+      <c r="C6" s="8">
+        <v>284911.45799999998</v>
       </c>
-      <c r="D6" s="4">
-        <f t="shared" si="0"/>
-        <v>76.25</v>
+      <c r="D6" s="8">
+        <v>2359.375</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:6" ht="15.75" thickBot="1">
       <c r="A7" s="1">
         <v>32000</v>
       </c>
-      <c r="B7" s="4">
-        <v>60</v>
+      <c r="B7" s="7">
+        <v>1037869.791</v>
       </c>
-      <c r="C7" s="4">
-        <f t="shared" si="1"/>
-        <v>1931.8899999999999</v>
+      <c r="C7" s="7">
+        <v>1090411.4580000001</v>
       </c>
-      <c r="D7" s="4">
-        <f t="shared" si="0"/>
-        <v>86.25</v>
+      <c r="D7" s="7">
+        <v>5244.7920000000004</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:6" ht="15.75" thickBot="1">
       <c r="A8" s="1">
         <v>64000</v>
       </c>
-      <c r="B8" s="4">
-        <v>70</v>
-      </c>
-      <c r="C8" s="4">
-        <f t="shared" si="1"/>
-        <v>3219.1499999999996</v>
-      </c>
-      <c r="D8" s="4">
-        <f t="shared" si="0"/>
-        <v>96.25</v>
+      <c r="B8" s="9"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="8">
+        <v>8495.625</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:6" ht="15.75" thickBot="1">
       <c r="A9" s="1">
         <v>128000</v>
       </c>
-      <c r="B9" s="4">
-        <v>80</v>
-      </c>
-      <c r="C9" s="4">
-        <f t="shared" si="1"/>
-        <v>5151.0399999999991</v>
-      </c>
-      <c r="D9" s="4">
-        <f t="shared" si="0"/>
-        <v>106.25</v>
+      <c r="B9" s="4"/>
+      <c r="C9" s="4"/>
+      <c r="D9" s="8">
+        <v>31187.5</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:6" ht="15.75" thickBot="1">
       <c r="A10" s="1">
         <v>256000</v>
       </c>
-      <c r="B10" s="4">
-        <v>90</v>
-      </c>
-      <c r="C10" s="4">
-        <f t="shared" si="1"/>
-        <v>8370.1899999999987</v>
-      </c>
-      <c r="D10" s="4">
-        <f t="shared" si="0"/>
-        <v>116.25</v>
+      <c r="B10" s="4"/>
+      <c r="C10" s="4"/>
+      <c r="D10" s="8">
+        <v>77869.792000000001</v>
       </c>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:6">
       <c r="A11" s="1">
         <v>512000</v>
       </c>
-      <c r="B11" s="4">
-        <v>100</v>
-      </c>
-      <c r="C11" s="4">
-        <f t="shared" si="1"/>
-        <v>13521.229999999998</v>
-      </c>
-      <c r="D11" s="4">
-        <f t="shared" si="0"/>
-        <v>126.25</v>
-      </c>
+      <c r="B11" s="4"/>
+      <c r="C11" s="4"/>
+      <c r="D11" s="4"/>
     </row>
-    <row r="14" spans="1:4">
+    <row r="12" spans="1:6">
+      <c r="F12" s="5"/>
+    </row>
+    <row r="14" spans="1:6" ht="30">
       <c r="A14" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:6" ht="15.75" thickBot="1">
       <c r="A15" s="1">
         <v>1000</v>
       </c>
-      <c r="B15" s="4">
-        <v>50</v>
+      <c r="B15" s="10">
+        <v>124432.291</v>
       </c>
-      <c r="C15" s="4">
-        <v>2</v>
+      <c r="C15" s="10">
+        <v>105270.833</v>
       </c>
-      <c r="D15" s="4">
-        <v>35</v>
+      <c r="D15" s="10">
+        <v>6380.2079999999996</v>
       </c>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16" spans="1:6" ht="16.5" thickTop="1" thickBot="1">
       <c r="A16" s="1">
         <v>2000</v>
       </c>
-      <c r="B16" s="4">
-        <v>60</v>
+      <c r="B16" s="7">
+        <v>630760.41599999997</v>
       </c>
-      <c r="C16" s="4">
-        <v>4</v>
+      <c r="C16" s="10">
+        <v>603000</v>
       </c>
-      <c r="D16" s="4">
-        <f>D15+43</f>
-        <v>78</v>
+      <c r="D16" s="7">
+        <v>25911.457999999999</v>
       </c>
     </row>
-    <row r="17" spans="1:4">
+    <row r="17" spans="1:4" ht="15.75" thickBot="1">
       <c r="A17" s="1">
         <v>4000</v>
       </c>
-      <c r="B17" s="4">
-        <v>70</v>
-      </c>
-      <c r="C17" s="4">
-        <f t="shared" ref="C17:C24" si="2">C16+C15</f>
-        <v>6</v>
-      </c>
-      <c r="D17" s="4">
-        <f t="shared" ref="D17:D24" si="3">D16+10</f>
-        <v>88</v>
+      <c r="B17" s="4"/>
+      <c r="C17" s="4"/>
+      <c r="D17" s="8">
+        <v>118604.167</v>
       </c>
     </row>
-    <row r="18" spans="1:4">
+    <row r="18" spans="1:4" ht="15.75" thickBot="1">
       <c r="A18" s="1">
         <v>8000</v>
       </c>
-      <c r="B18" s="4">
-        <v>80</v>
-      </c>
-      <c r="C18" s="4">
-        <f t="shared" si="2"/>
-        <v>10</v>
-      </c>
-      <c r="D18" s="4">
-        <f t="shared" si="3"/>
-        <v>98</v>
+      <c r="B18" s="4"/>
+      <c r="C18" s="4"/>
+      <c r="D18" s="7">
+        <v>583630.20799999998</v>
       </c>
     </row>
     <row r="19" spans="1:4">
       <c r="A19" s="1">
         <v>16000</v>
       </c>
-      <c r="B19" s="4">
-        <v>90</v>
-      </c>
-      <c r="C19" s="4">
-        <f t="shared" si="2"/>
-        <v>16</v>
-      </c>
-      <c r="D19" s="4">
-        <f t="shared" si="3"/>
-        <v>108</v>
-      </c>
+      <c r="B19" s="4"/>
+      <c r="C19" s="4"/>
+      <c r="D19" s="4"/>
     </row>
     <row r="20" spans="1:4">
       <c r="A20" s="1">
         <v>32000</v>
       </c>
-      <c r="B20" s="4">
-        <v>100</v>
-      </c>
-      <c r="C20" s="4">
-        <f t="shared" si="2"/>
-        <v>26</v>
-      </c>
-      <c r="D20" s="4">
-        <f t="shared" si="3"/>
-        <v>118</v>
-      </c>
+      <c r="B20" s="4"/>
+      <c r="C20" s="4"/>
+      <c r="D20" s="4"/>
     </row>
     <row r="21" spans="1:4">
       <c r="A21" s="1">
         <v>64000</v>
       </c>
-      <c r="B21" s="4">
-        <v>110</v>
-      </c>
-      <c r="C21" s="4">
-        <f t="shared" si="2"/>
-        <v>42</v>
-      </c>
-      <c r="D21" s="4">
-        <f t="shared" si="3"/>
-        <v>128</v>
-      </c>
+      <c r="B21" s="4"/>
+      <c r="C21" s="4"/>
+      <c r="D21" s="4"/>
     </row>
     <row r="22" spans="1:4">
       <c r="A22" s="1">
         <v>128000</v>
       </c>
-      <c r="B22" s="4">
-        <v>120</v>
-      </c>
-      <c r="C22" s="4">
-        <f t="shared" si="2"/>
-        <v>68</v>
-      </c>
-      <c r="D22" s="4">
-        <f t="shared" si="3"/>
-        <v>138</v>
-      </c>
+      <c r="B22" s="4"/>
+      <c r="C22" s="4"/>
+      <c r="D22" s="4"/>
     </row>
     <row r="23" spans="1:4">
       <c r="A23" s="1">
         <v>256000</v>
       </c>
-      <c r="B23" s="4">
-        <v>130</v>
-      </c>
-      <c r="C23" s="4">
-        <f t="shared" si="2"/>
-        <v>110</v>
-      </c>
-      <c r="D23" s="4">
-        <f t="shared" si="3"/>
-        <v>148</v>
-      </c>
+      <c r="B23" s="4"/>
+      <c r="C23" s="4"/>
+      <c r="D23" s="4"/>
     </row>
     <row r="24" spans="1:4">
       <c r="A24" s="1">
         <v>512000</v>
       </c>
-      <c r="B24" s="4">
-        <v>140</v>
-      </c>
-      <c r="C24" s="4">
-        <f t="shared" si="2"/>
-        <v>178</v>
-      </c>
-      <c r="D24" s="4">
-        <f t="shared" si="3"/>
-        <v>158</v>
-      </c>
+      <c r="B24" s="4"/>
+      <c r="C24" s="4"/>
+      <c r="D24" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -8191,9 +8057,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -8408,19 +8277,15 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{97C5E1E0-C817-4769-9D2D-1DC296B681FA}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F8DF3742-38F2-4B99-B335-CC4F04ED9F45}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -8445,9 +8310,10 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F8DF3742-38F2-4B99-B335-CC4F04ED9F45}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{97C5E1E0-C817-4769-9D2D-1DC296B681FA}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>